<commit_message>
Prepare readme with howto & examples Minor change to xlsx template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/xls/default.xlsx
+++ b/src/main/resources/templates/xls/default.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F8C19A-D405-E446-A1C2-E2A17FD15FE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC5D936-0A76-FD44-B8F0-BFD6C7F607CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="21800" windowHeight="13540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,13 +62,16 @@
     <t>Simple XLSX Example</t>
   </si>
   <si>
-    <t>${employee.age} Jahre</t>
+    <t>${employee.age} yr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,18 +146,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -515,27 +516,27 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="4" customWidth="1"/>
     <col min="3" max="4" width="17.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="255" width="8.83203125" style="6" customWidth="1"/>
-    <col min="256" max="16384" width="10.83203125" style="6"/>
+    <col min="6" max="255" width="8.83203125" style="4" customWidth="1"/>
+    <col min="256" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -545,13 +546,13 @@
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -559,28 +560,28 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <f>SUM(D4)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <f>SUM(E4)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Refactored loading template resources ExcelService uses fileTemplateLoader to load resources
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/xls/default.xlsx
+++ b/src/main/resources/templates/xls/default.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC5D936-0A76-FD44-B8F0-BFD6C7F607CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380FA6F8-EFA0-AD48-B1EE-FDF9EF3425C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="21800" windowHeight="13540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added multi sheet support
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/xls/default.xlsx
+++ b/src/main/resources/templates/xls/default.xlsx
@@ -3,15 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380FA6F8-EFA0-AD48-B1EE-FDF9EF3425C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7817A8D0-F4FF-4040-85EB-A633DF14A055}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="21800" windowHeight="13540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="21800" windowHeight="13540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Result" sheetId="2" r:id="rId1"/>
-    <sheet name="Template" sheetId="1" r:id="rId2"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -495,23 +494,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="256" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>

</xml_diff>